<commit_message>
Move hh_snake_bites into hh_member
</commit_message>
<xml_diff>
--- a/odkx/forms/hh_member.xlsx
+++ b/odkx/forms/hh_member.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="503">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -383,6 +383,60 @@
     <t xml:space="preserve">Hang out with friends or relatives </t>
   </si>
   <si>
+    <t xml:space="preserve">bite_occur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inside the home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inside the compound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bite_outcome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">death</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Death</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loss_limb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loss of limb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">full_recovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full recovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">partial_recovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partial recovery</t>
+  </si>
+  <si>
     <t xml:space="preserve">breastfeed</t>
   </si>
   <si>
@@ -749,6 +803,81 @@
     <t xml:space="preserve">He/she emigrated</t>
   </si>
   <si>
+    <t xml:space="preserve">month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">january</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January</t>
+  </si>
+  <si>
+    <t xml:space="preserve">february</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February</t>
+  </si>
+  <si>
+    <t xml:space="preserve">march</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March</t>
+  </si>
+  <si>
+    <t xml:space="preserve">april</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April</t>
+  </si>
+  <si>
+    <t xml:space="preserve">may</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May</t>
+  </si>
+  <si>
+    <t xml:space="preserve">june</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June</t>
+  </si>
+  <si>
+    <t xml:space="preserve">july</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July</t>
+  </si>
+  <si>
+    <t xml:space="preserve">august</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August</t>
+  </si>
+  <si>
+    <t xml:space="preserve">september</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September</t>
+  </si>
+  <si>
+    <t xml:space="preserve">october</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October</t>
+  </si>
+  <si>
+    <t xml:space="preserve">november</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November</t>
+  </si>
+  <si>
+    <t xml:space="preserve">december</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December</t>
+  </si>
+  <si>
     <t xml:space="preserve">new_member</t>
   </si>
   <si>
@@ -1203,6 +1332,33 @@
   </si>
   <si>
     <t xml:space="preserve">new_hh_member_censed_extid_not_possible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snake Bites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snake_bite_num_times</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snake_bite_months</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snake_bite_miss_work_school</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snake_bite_miss_work_school_days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snake_bite_miss_work_school_days_unknown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snake_bite_occur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snake_bite_occur_other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snake_bite_outcome</t>
   </si>
   <si>
     <t xml:space="preserve">Individual Questionnaire</t>
@@ -1445,7 +1601,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1480,6 +1636,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDE8CB"/>
         <bgColor rgb="FFDEE6EF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6F9D4"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -1523,7 +1685,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1568,7 +1730,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1601,7 +1767,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFF6F9D4"/>
       <rgbColor rgb="FFDEE6EF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -1652,10 +1818,10 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:C4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.62890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="8.7"/>
   </cols>
@@ -2703,10 +2869,10 @@
   <dimension ref="A1:K998"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:C4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.62890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.4"/>
@@ -4018,14 +4184,14 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A16" activeCellId="1" sqref="B4:C4 A16"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.62890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="4" style="0" width="11.39"/>
   </cols>
   <sheetData>
@@ -4846,73 +5012,73 @@
         <v>119</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>61</v>
+        <v>124</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>61</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>127</v>
+        <v>89</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>127</v>
+        <v>90</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>128</v>
+        <v>27</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>129</v>
+        <v>54</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B60" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="C60" s="0" t="s">
         <v>130</v>
-      </c>
-      <c r="C60" s="0" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B61" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="C61" s="0" t="s">
         <v>132</v>
-      </c>
-      <c r="C61" s="0" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C62" s="0" t="s">
         <v>134</v>
@@ -4920,244 +5086,244 @@
     </row>
     <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B63" s="0" t="s">
         <v>135</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>138</v>
+        <v>61</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>139</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>64</v>
+        <v>148</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>65</v>
+        <v>149</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>89</v>
+        <v>150</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>90</v>
+        <v>151</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>64</v>
+        <v>161</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>65</v>
+        <v>161</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>156</v>
+        <v>89</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>157</v>
+        <v>90</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>27</v>
+        <v>165</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>54</v>
+        <v>166</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5165,10 +5331,10 @@
         <v>162</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5176,10 +5342,10 @@
         <v>162</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5187,10 +5353,10 @@
         <v>162</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5198,62 +5364,62 @@
         <v>162</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>172</v>
+        <v>64</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>173</v>
+        <v>65</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>174</v>
+        <v>89</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>174</v>
+        <v>90</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B91" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="C91" s="0" t="s">
         <v>175</v>
-      </c>
-      <c r="C91" s="0" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B92" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="C92" s="0" t="s">
         <v>177</v>
-      </c>
-      <c r="C92" s="0" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C93" s="0" t="s">
         <v>179</v>
@@ -5261,62 +5427,62 @@
     </row>
     <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>180</v>
+        <v>27</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>181</v>
+        <v>54</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="B95" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="C95" s="0" t="s">
         <v>182</v>
-      </c>
-      <c r="C95" s="0" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="B96" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="C96" s="0" t="s">
         <v>184</v>
-      </c>
-      <c r="C96" s="0" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="B97" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="C97" s="0" t="s">
         <v>186</v>
-      </c>
-      <c r="C97" s="0" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>43</v>
+        <v>180</v>
       </c>
       <c r="B98" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="C98" s="0" t="s">
         <v>188</v>
-      </c>
-      <c r="C98" s="0" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>43</v>
+        <v>189</v>
       </c>
       <c r="B99" s="0" t="s">
         <v>190</v>
@@ -5327,54 +5493,54 @@
     </row>
     <row r="100" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="B100" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="B100" s="0" t="s">
-        <v>193</v>
-      </c>
       <c r="C100" s="0" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>27</v>
+        <v>195</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>54</v>
+        <v>196</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="B103" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="B103" s="0" t="s">
-        <v>198</v>
-      </c>
       <c r="C103" s="0" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C104" s="0" t="s">
         <v>199</v>
@@ -5382,802 +5548,802 @@
     </row>
     <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B105" s="0" t="s">
         <v>200</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>197</v>
+        <v>43</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>197</v>
+        <v>43</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>207</v>
+        <v>27</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>207</v>
+        <v>54</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>197</v>
+        <v>215</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>27</v>
+        <v>216</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>197</v>
+        <v>215</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>64</v>
+        <v>217</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>65</v>
+        <v>217</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>197</v>
+        <v>215</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>89</v>
+        <v>218</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>90</v>
+        <v>218</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>61</v>
+        <v>223</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>61</v>
+        <v>223</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>27</v>
+        <v>224</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>54</v>
+        <v>224</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>217</v>
+        <v>27</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="B126" s="0" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="B128" s="0" t="s">
-        <v>27</v>
+        <v>230</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>208</v>
+        <v>230</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="B130" s="0" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B131" s="0" t="s">
-        <v>227</v>
+        <v>27</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>227</v>
+        <v>54</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B132" s="0" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B133" s="0" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B134" s="0" t="s">
-        <v>230</v>
+        <v>60</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>230</v>
+        <v>61</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B135" s="0" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="B136" s="0" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="B137" s="0" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="B138" s="0" t="s">
-        <v>234</v>
+        <v>27</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="B139" s="0" t="s">
-        <v>27</v>
+        <v>242</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B140" s="0" t="s">
-        <v>237</v>
+        <v>64</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>238</v>
+        <v>65</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="B141" s="0" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B142" s="0" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B143" s="0" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B144" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B145" s="0" t="s">
-        <v>125</v>
+        <v>27</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>126</v>
+        <v>88</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B146" s="0" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B147" s="0" t="s">
-        <v>127</v>
+        <v>251</v>
       </c>
       <c r="C147" s="0" t="s">
-        <v>127</v>
+        <v>251</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B148" s="0" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="C148" s="0" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B149" s="0" t="s">
-        <v>128</v>
+        <v>27</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>129</v>
+        <v>253</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="B150" s="0" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="C150" s="0" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="B151" s="0" t="s">
-        <v>130</v>
+        <v>257</v>
       </c>
       <c r="C151" s="0" t="s">
-        <v>131</v>
+        <v>258</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
       <c r="B152" s="0" t="s">
-        <v>134</v>
+        <v>260</v>
       </c>
       <c r="C152" s="0" t="s">
-        <v>134</v>
+        <v>261</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
       <c r="B153" s="0" t="s">
-        <v>89</v>
+        <v>262</v>
       </c>
       <c r="C153" s="0" t="s">
-        <v>90</v>
+        <v>263</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="B154" s="0" t="s">
-        <v>249</v>
+        <v>264</v>
       </c>
       <c r="C154" s="0" t="s">
-        <v>249</v>
+        <v>265</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="B155" s="0" t="s">
-        <v>253</v>
+        <v>266</v>
       </c>
       <c r="C155" s="0" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="B156" s="0" t="s">
-        <v>254</v>
+        <v>268</v>
       </c>
       <c r="C156" s="0" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="B157" s="0" t="s">
-        <v>255</v>
+        <v>270</v>
       </c>
       <c r="C157" s="0" t="s">
-        <v>256</v>
+        <v>271</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="B158" s="0" t="s">
-        <v>257</v>
+        <v>272</v>
       </c>
       <c r="C158" s="0" t="s">
-        <v>257</v>
+        <v>273</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="B159" s="0" t="s">
-        <v>258</v>
+        <v>274</v>
       </c>
       <c r="C159" s="0" t="s">
-        <v>258</v>
+        <v>275</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="B160" s="0" t="s">
-        <v>127</v>
+        <v>276</v>
       </c>
       <c r="C160" s="0" t="s">
-        <v>127</v>
+        <v>277</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="B161" s="0" t="s">
-        <v>259</v>
+        <v>278</v>
       </c>
       <c r="C161" s="0" t="s">
-        <v>260</v>
+        <v>279</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="B162" s="0" t="s">
-        <v>261</v>
+        <v>280</v>
       </c>
       <c r="C162" s="0" t="s">
-        <v>262</v>
+        <v>281</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="B163" s="0" t="s">
-        <v>89</v>
+        <v>282</v>
       </c>
       <c r="C163" s="0" t="s">
-        <v>90</v>
+        <v>283</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B164" s="0" t="s">
-        <v>264</v>
+        <v>27</v>
       </c>
       <c r="C164" s="0" t="s">
-        <v>265</v>
+        <v>54</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>263</v>
+        <v>284</v>
       </c>
       <c r="B165" s="0" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="C165" s="0" t="s">
-        <v>267</v>
+        <v>286</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>263</v>
+        <v>284</v>
       </c>
       <c r="B166" s="0" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="C166" s="0" t="s">
-        <v>269</v>
+        <v>288</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>263</v>
+        <v>289</v>
       </c>
       <c r="B167" s="0" t="s">
-        <v>270</v>
+        <v>290</v>
       </c>
       <c r="C167" s="0" t="s">
-        <v>271</v>
+        <v>290</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>272</v>
+        <v>289</v>
       </c>
       <c r="B168" s="0" t="s">
-        <v>273</v>
+        <v>143</v>
       </c>
       <c r="C168" s="0" t="s">
-        <v>274</v>
+        <v>144</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>272</v>
+        <v>289</v>
       </c>
       <c r="B169" s="0" t="s">
-        <v>275</v>
+        <v>291</v>
       </c>
       <c r="C169" s="0" t="s">
-        <v>276</v>
+        <v>291</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>272</v>
+        <v>289</v>
       </c>
       <c r="B170" s="0" t="s">
-        <v>277</v>
+        <v>145</v>
       </c>
       <c r="C170" s="0" t="s">
-        <v>278</v>
+        <v>145</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>272</v>
+        <v>289</v>
       </c>
       <c r="B171" s="0" t="s">
-        <v>279</v>
+        <v>292</v>
       </c>
       <c r="C171" s="0" t="s">
-        <v>280</v>
+        <v>292</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>272</v>
+        <v>289</v>
       </c>
       <c r="B172" s="0" t="s">
-        <v>281</v>
+        <v>146</v>
       </c>
       <c r="C172" s="0" t="s">
-        <v>282</v>
+        <v>147</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>272</v>
+        <v>289</v>
       </c>
       <c r="B173" s="0" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="C173" s="0" t="s">
-        <v>284</v>
+        <v>294</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>272</v>
+        <v>289</v>
       </c>
       <c r="B174" s="0" t="s">
-        <v>285</v>
+        <v>148</v>
       </c>
       <c r="C174" s="0" t="s">
-        <v>286</v>
+        <v>149</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>272</v>
+        <v>289</v>
       </c>
       <c r="B175" s="0" t="s">
-        <v>287</v>
+        <v>152</v>
       </c>
       <c r="C175" s="0" t="s">
-        <v>288</v>
+        <v>152</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>272</v>
+        <v>289</v>
       </c>
       <c r="B176" s="0" t="s">
-        <v>289</v>
+        <v>89</v>
       </c>
       <c r="C176" s="0" t="s">
-        <v>290</v>
+        <v>90</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>272</v>
+        <v>295</v>
       </c>
       <c r="B177" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C177" s="0" t="s">
         <v>292</v>
@@ -6185,131 +6351,131 @@
     </row>
     <row r="178" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>272</v>
+        <v>295</v>
       </c>
       <c r="B178" s="0" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="C178" s="0" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>272</v>
+        <v>295</v>
       </c>
       <c r="B179" s="0" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="C179" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>272</v>
+        <v>295</v>
       </c>
       <c r="B180" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C180" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>272</v>
+        <v>295</v>
       </c>
       <c r="B181" s="0" t="s">
-        <v>89</v>
+        <v>300</v>
       </c>
       <c r="C181" s="0" t="s">
-        <v>90</v>
+        <v>300</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>45</v>
+        <v>295</v>
       </c>
       <c r="B182" s="0" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="C182" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>45</v>
+        <v>295</v>
       </c>
       <c r="B183" s="0" t="s">
-        <v>301</v>
+        <v>145</v>
       </c>
       <c r="C183" s="0" t="s">
-        <v>302</v>
+        <v>145</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="B184" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="C184" s="0" t="s">
         <v>303</v>
-      </c>
-      <c r="B184" s="0" t="s">
-        <v>304</v>
-      </c>
-      <c r="C184" s="0" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="B185" s="0" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C185" s="0" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="B186" s="0" t="s">
-        <v>309</v>
+        <v>89</v>
       </c>
       <c r="C186" s="0" t="s">
-        <v>309</v>
+        <v>90</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="B187" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="C187" s="0" t="s">
         <v>308</v>
-      </c>
-      <c r="B187" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="C187" s="0" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B188" s="0" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C188" s="0" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B189" s="0" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C189" s="0" t="s">
         <v>312</v>
@@ -6317,10 +6483,10 @@
     </row>
     <row r="190" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="B190" s="0" t="s">
         <v>313</v>
-      </c>
-      <c r="B190" s="0" t="s">
-        <v>314</v>
       </c>
       <c r="C190" s="0" t="s">
         <v>314</v>
@@ -6328,489 +6494,719 @@
     </row>
     <row r="191" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B191" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C191" s="0" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B192" s="0" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C192" s="0" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B193" s="0" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="C193" s="0" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B194" s="0" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="C194" s="0" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B195" s="0" t="s">
-        <v>314</v>
+        <v>324</v>
       </c>
       <c r="C195" s="0" t="s">
-        <v>314</v>
+        <v>325</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B196" s="0" t="s">
-        <v>315</v>
+        <v>326</v>
       </c>
       <c r="C196" s="0" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B197" s="0" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
       <c r="C197" s="0" t="s">
-        <v>316</v>
+        <v>329</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B198" s="0" t="s">
-        <v>317</v>
+        <v>330</v>
       </c>
       <c r="C198" s="0" t="s">
-        <v>317</v>
+        <v>331</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B199" s="0" t="s">
-        <v>318</v>
+        <v>332</v>
       </c>
       <c r="C199" s="0" t="s">
-        <v>318</v>
+        <v>333</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="B200" s="0" t="s">
-        <v>309</v>
+        <v>334</v>
       </c>
       <c r="C200" s="0" t="s">
-        <v>309</v>
+        <v>335</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="B201" s="0" t="s">
-        <v>310</v>
+        <v>336</v>
       </c>
       <c r="C201" s="0" t="s">
-        <v>310</v>
+        <v>337</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="B202" s="0" t="s">
-        <v>311</v>
+        <v>338</v>
       </c>
       <c r="C202" s="0" t="s">
-        <v>311</v>
+        <v>339</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="B203" s="0" t="s">
-        <v>312</v>
+        <v>340</v>
       </c>
       <c r="C203" s="0" t="s">
-        <v>312</v>
+        <v>341</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="B204" s="0" t="s">
-        <v>322</v>
+        <v>89</v>
       </c>
       <c r="C204" s="0" t="s">
-        <v>322</v>
+        <v>90</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>321</v>
+        <v>45</v>
       </c>
       <c r="B205" s="0" t="s">
-        <v>323</v>
+        <v>342</v>
       </c>
       <c r="C205" s="0" t="s">
-        <v>323</v>
+        <v>343</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>321</v>
+        <v>45</v>
       </c>
       <c r="B206" s="0" t="s">
-        <v>324</v>
+        <v>344</v>
       </c>
       <c r="C206" s="0" t="s">
-        <v>324</v>
+        <v>345</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>321</v>
+        <v>346</v>
       </c>
       <c r="B207" s="0" t="s">
-        <v>325</v>
+        <v>347</v>
       </c>
       <c r="C207" s="0" t="s">
-        <v>326</v>
+        <v>348</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>321</v>
+        <v>346</v>
       </c>
       <c r="B208" s="0" t="s">
-        <v>327</v>
+        <v>349</v>
       </c>
       <c r="C208" s="0" t="s">
-        <v>327</v>
+        <v>350</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>321</v>
+        <v>351</v>
       </c>
       <c r="B209" s="0" t="s">
-        <v>328</v>
+        <v>352</v>
       </c>
       <c r="C209" s="0" t="s">
-        <v>329</v>
+        <v>352</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
-        <v>321</v>
+        <v>351</v>
       </c>
       <c r="B210" s="0" t="s">
-        <v>330</v>
+        <v>353</v>
       </c>
       <c r="C210" s="0" t="s">
-        <v>330</v>
+        <v>353</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>321</v>
+        <v>351</v>
       </c>
       <c r="B211" s="0" t="s">
-        <v>331</v>
+        <v>354</v>
       </c>
       <c r="C211" s="0" t="s">
-        <v>331</v>
+        <v>354</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>321</v>
+        <v>351</v>
       </c>
       <c r="B212" s="0" t="s">
-        <v>332</v>
+        <v>355</v>
       </c>
       <c r="C212" s="0" t="s">
-        <v>332</v>
+        <v>355</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>321</v>
+        <v>356</v>
       </c>
       <c r="B213" s="0" t="s">
-        <v>333</v>
+        <v>357</v>
       </c>
       <c r="C213" s="0" t="s">
-        <v>333</v>
+        <v>357</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>321</v>
+        <v>356</v>
       </c>
       <c r="B214" s="0" t="s">
-        <v>153</v>
+        <v>358</v>
       </c>
       <c r="C214" s="0" t="s">
-        <v>154</v>
+        <v>358</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>334</v>
+        <v>356</v>
       </c>
       <c r="B215" s="0" t="s">
-        <v>335</v>
+        <v>359</v>
       </c>
       <c r="C215" s="0" t="s">
-        <v>336</v>
+        <v>359</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>334</v>
+        <v>356</v>
       </c>
       <c r="B216" s="0" t="s">
-        <v>337</v>
+        <v>360</v>
       </c>
       <c r="C216" s="0" t="s">
-        <v>337</v>
+        <v>360</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
-        <v>334</v>
+        <v>356</v>
       </c>
       <c r="B217" s="0" t="s">
-        <v>338</v>
+        <v>361</v>
       </c>
       <c r="C217" s="0" t="s">
-        <v>339</v>
+        <v>361</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>334</v>
+        <v>362</v>
       </c>
       <c r="B218" s="0" t="s">
-        <v>340</v>
+        <v>357</v>
       </c>
       <c r="C218" s="0" t="s">
-        <v>340</v>
+        <v>357</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
-        <v>334</v>
+        <v>362</v>
       </c>
       <c r="B219" s="0" t="s">
-        <v>341</v>
+        <v>358</v>
       </c>
       <c r="C219" s="0" t="s">
-        <v>341</v>
+        <v>358</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>334</v>
+        <v>362</v>
       </c>
       <c r="B220" s="0" t="s">
-        <v>342</v>
+        <v>359</v>
       </c>
       <c r="C220" s="0" t="s">
-        <v>343</v>
+        <v>359</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
-        <v>334</v>
+        <v>362</v>
       </c>
       <c r="B221" s="0" t="s">
-        <v>344</v>
+        <v>360</v>
       </c>
       <c r="C221" s="0" t="s">
-        <v>344</v>
+        <v>360</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>334</v>
+        <v>362</v>
       </c>
       <c r="B222" s="0" t="s">
-        <v>345</v>
+        <v>361</v>
       </c>
       <c r="C222" s="0" t="s">
-        <v>346</v>
+        <v>361</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>334</v>
+        <v>363</v>
       </c>
       <c r="B223" s="0" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="C223" s="0" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
-        <v>334</v>
+        <v>363</v>
       </c>
       <c r="B224" s="0" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="C224" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>334</v>
+        <v>363</v>
       </c>
       <c r="B225" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="C225" s="0" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>334</v>
+        <v>363</v>
       </c>
       <c r="B226" s="0" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="C226" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>334</v>
+        <v>364</v>
       </c>
       <c r="B227" s="0" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="C227" s="0" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
-        <v>334</v>
+        <v>364</v>
       </c>
       <c r="B228" s="0" t="s">
-        <v>357</v>
+        <v>366</v>
       </c>
       <c r="C228" s="0" t="s">
-        <v>358</v>
+        <v>366</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
-        <v>334</v>
+        <v>364</v>
       </c>
       <c r="B229" s="0" t="s">
-        <v>27</v>
+        <v>367</v>
       </c>
       <c r="C229" s="0" t="s">
-        <v>88</v>
+        <v>367</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
-        <v>334</v>
+        <v>364</v>
       </c>
       <c r="B230" s="0" t="s">
-        <v>64</v>
+        <v>368</v>
       </c>
       <c r="C230" s="0" t="s">
-        <v>359</v>
+        <v>369</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
-        <v>334</v>
+        <v>364</v>
       </c>
       <c r="B231" s="0" t="s">
-        <v>89</v>
+        <v>370</v>
       </c>
       <c r="C231" s="0" t="s">
-        <v>90</v>
+        <v>370</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>334</v>
+        <v>364</v>
       </c>
       <c r="B232" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="C232" s="0" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="233" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A233" s="0" t="s">
+        <v>364</v>
+      </c>
+      <c r="B233" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="C233" s="0" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="234" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A234" s="0" t="s">
+        <v>364</v>
+      </c>
+      <c r="B234" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="C234" s="0" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A235" s="0" t="s">
+        <v>364</v>
+      </c>
+      <c r="B235" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="C235" s="0" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="236" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A236" s="0" t="s">
+        <v>364</v>
+      </c>
+      <c r="B236" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="C236" s="0" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="237" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A237" s="0" t="s">
+        <v>364</v>
+      </c>
+      <c r="B237" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="C237" s="0" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="238" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A238" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B238" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="C238" s="0" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A239" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B239" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="C239" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A240" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B240" s="0" t="s">
+        <v>381</v>
+      </c>
+      <c r="C240" s="0" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="241" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A241" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B241" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="C241" s="0" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="242" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A242" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B242" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="C242" s="0" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="243" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A243" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B243" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="C243" s="0" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="244" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A244" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B244" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="C244" s="0" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="245" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A245" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B245" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="C245" s="0" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A246" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B246" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="C246" s="0" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A247" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B247" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="C247" s="0" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="248" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A248" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B248" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="C248" s="0" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A249" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B249" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="C249" s="0" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="250" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A250" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B250" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="C250" s="0" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="251" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A251" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B251" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="C251" s="0" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="252" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A252" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B252" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C252" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="253" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A253" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B253" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C253" s="0" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="254" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A254" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B254" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C254" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="255" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A255" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B255" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C232" s="0" t="s">
+      <c r="C255" s="0" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="233" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="234" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="235" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="236" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="237" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="238" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="239" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="240" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="241" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="242" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="243" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="244" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="245" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="246" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="247" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="248" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="249" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="250" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="251" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="252" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="253" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="254" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="255" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="256" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="257" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="258" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -7583,13 +7979,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y747"/>
+  <dimension ref="A1:Y755"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4:C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.62890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.79"/>
@@ -7600,7 +7996,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>360</v>
+        <v>403</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>9</v>
@@ -7609,7 +8005,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>361</v>
+        <v>404</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -7635,13 +8031,13 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>362</v>
+        <v>405</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>363</v>
+        <v>406</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>364</v>
+        <v>407</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -7667,10 +8063,10 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="6" t="s">
-        <v>365</v>
+        <v>408</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>364</v>
+        <v>407</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -7696,10 +8092,10 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="6" t="s">
-        <v>366</v>
+        <v>409</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>364</v>
+        <v>407</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -7725,7 +8121,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>367</v>
+        <v>410</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>9</v>
@@ -8123,16 +8519,16 @@
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>368</v>
+        <v>411</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>369</v>
+        <v>412</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>42</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>303</v>
+        <v>346</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -8158,10 +8554,10 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="8" t="s">
-        <v>370</v>
+        <v>413</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>371</v>
+        <v>414</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -8187,7 +8583,7 @@
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="8" t="s">
-        <v>372</v>
+        <v>415</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>22</v>
@@ -8216,13 +8612,13 @@
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="8" t="s">
-        <v>373</v>
+        <v>416</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>42</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -8248,7 +8644,7 @@
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="8" t="s">
-        <v>374</v>
+        <v>417</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>26</v>
@@ -8312,16 +8708,16 @@
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>375</v>
+        <v>418</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>236</v>
+        <v>254</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>42</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>236</v>
+        <v>254</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -8347,10 +8743,10 @@
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="9" t="s">
-        <v>376</v>
+        <v>419</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>371</v>
+        <v>414</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -8376,7 +8772,7 @@
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="9" t="s">
-        <v>377</v>
+        <v>420</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>26</v>
@@ -8408,10 +8804,10 @@
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="9" t="s">
-        <v>378</v>
+        <v>421</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>371</v>
+        <v>414</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -8437,7 +8833,7 @@
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="9" t="s">
-        <v>379</v>
+        <v>422</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>22</v>
@@ -8466,13 +8862,13 @@
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="9" t="s">
-        <v>380</v>
+        <v>423</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>42</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
@@ -8498,13 +8894,13 @@
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="9" t="s">
-        <v>381</v>
+        <v>424</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>42</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
@@ -8530,16 +8926,16 @@
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>382</v>
+        <v>425</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>383</v>
+        <v>426</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>42</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>241</v>
+        <v>284</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
@@ -8565,10 +8961,10 @@
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B32" s="10" t="s">
-        <v>384</v>
+        <v>427</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>371</v>
+        <v>414</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
@@ -8594,7 +8990,7 @@
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="10" t="s">
-        <v>385</v>
+        <v>428</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>22</v>
@@ -8623,13 +9019,13 @@
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B34" s="10" t="s">
-        <v>386</v>
+        <v>429</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>42</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
@@ -8655,13 +9051,13 @@
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="10" t="s">
-        <v>387</v>
+        <v>430</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>42</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
@@ -8687,7 +9083,7 @@
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B36" s="10" t="s">
-        <v>388</v>
+        <v>431</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>42</v>
@@ -8719,7 +9115,7 @@
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B37" s="10" t="s">
-        <v>389</v>
+        <v>432</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>26</v>
@@ -8751,10 +9147,10 @@
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>390</v>
+        <v>433</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>391</v>
+        <v>434</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>42</v>
@@ -8786,7 +9182,7 @@
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B39" s="7" t="s">
-        <v>392</v>
+        <v>435</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>26</v>
@@ -8818,16 +9214,13 @@
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>393</v>
+        <v>436</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>394</v>
+        <v>437</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
@@ -8853,13 +9246,13 @@
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B41" s="11" t="s">
-        <v>395</v>
+        <v>438</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>57</v>
+        <v>259</v>
       </c>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
@@ -8885,13 +9278,13 @@
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B42" s="11" t="s">
-        <v>396</v>
+        <v>439</v>
       </c>
       <c r="C42" s="11" t="s">
         <v>42</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
@@ -8917,10 +9310,10 @@
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B43" s="11" t="s">
-        <v>397</v>
+        <v>440</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>398</v>
+        <v>22</v>
       </c>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
@@ -8946,13 +9339,13 @@
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B44" s="11" t="s">
-        <v>399</v>
+        <v>441</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
@@ -8978,10 +9371,13 @@
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B45" s="11" t="s">
-        <v>400</v>
+        <v>442</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>398</v>
+        <v>26</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>119</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
@@ -9007,10 +9403,10 @@
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B46" s="11" t="s">
-        <v>401</v>
+        <v>443</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>398</v>
+        <v>16</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
@@ -9036,13 +9432,13 @@
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="11" t="s">
-        <v>402</v>
+        <v>444</v>
       </c>
       <c r="C47" s="11" t="s">
         <v>42</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>263</v>
+        <v>128</v>
       </c>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
@@ -9067,14 +9463,17 @@
       <c r="Y47" s="5"/>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="11" t="s">
-        <v>403</v>
-      </c>
-      <c r="C48" s="11" t="s">
+      <c r="A48" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>446</v>
+      </c>
+      <c r="C48" s="12" t="s">
         <v>42</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>272</v>
+        <v>57</v>
       </c>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
@@ -9099,14 +9498,14 @@
       <c r="Y48" s="5"/>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B49" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="C49" s="11" t="s">
+      <c r="B49" s="12" t="s">
+        <v>447</v>
+      </c>
+      <c r="C49" s="12" t="s">
         <v>42</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>197</v>
+        <v>57</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
@@ -9131,14 +9530,14 @@
       <c r="Y49" s="5"/>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B50" s="11" t="s">
-        <v>404</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>405</v>
+      <c r="B50" s="12" t="s">
+        <v>448</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>406</v>
+        <v>57</v>
       </c>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
@@ -9163,14 +9562,11 @@
       <c r="Y50" s="5"/>
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B51" s="11" t="s">
-        <v>407</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D51" s="0" t="s">
-        <v>334</v>
+      <c r="B51" s="12" t="s">
+        <v>449</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>450</v>
       </c>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
@@ -9195,14 +9591,14 @@
       <c r="Y51" s="5"/>
     </row>
     <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="11" t="s">
-        <v>408</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>26</v>
+      <c r="B52" s="12" t="s">
+        <v>451</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>124</v>
+        <v>57</v>
       </c>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
@@ -9227,11 +9623,11 @@
       <c r="Y52" s="5"/>
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B53" s="11" t="s">
-        <v>409</v>
-      </c>
-      <c r="C53" s="11" t="s">
-        <v>16</v>
+      <c r="B53" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>450</v>
       </c>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
@@ -9256,14 +9652,11 @@
       <c r="Y53" s="5"/>
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B54" s="11" t="s">
-        <v>410</v>
-      </c>
-      <c r="C54" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D54" s="0" t="s">
-        <v>62</v>
+      <c r="B54" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>450</v>
       </c>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
@@ -9288,14 +9681,14 @@
       <c r="Y54" s="5"/>
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B55" s="11" t="s">
-        <v>411</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>26</v>
+      <c r="B55" s="12" t="s">
+        <v>454</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>246</v>
+        <v>306</v>
       </c>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
@@ -9320,11 +9713,14 @@
       <c r="Y55" s="5"/>
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B56" s="11" t="s">
-        <v>412</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>16</v>
+      <c r="B56" s="12" t="s">
+        <v>455</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>315</v>
       </c>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
@@ -9349,14 +9745,14 @@
       <c r="Y56" s="5"/>
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B57" s="11" t="s">
-        <v>413</v>
-      </c>
-      <c r="C57" s="11" t="s">
-        <v>26</v>
+      <c r="B57" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>252</v>
+        <v>215</v>
       </c>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
@@ -9381,11 +9777,14 @@
       <c r="Y57" s="5"/>
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B58" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="C58" s="11" t="s">
-        <v>16</v>
+      <c r="B58" s="12" t="s">
+        <v>456</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>457</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>458</v>
       </c>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
@@ -9410,14 +9809,14 @@
       <c r="Y58" s="5"/>
     </row>
     <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B59" s="11" t="s">
-        <v>415</v>
-      </c>
-      <c r="C59" s="11" t="s">
-        <v>42</v>
+      <c r="B59" s="12" t="s">
+        <v>459</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>57</v>
+        <v>377</v>
       </c>
       <c r="E59" s="5"/>
       <c r="F59" s="5"/>
@@ -9442,14 +9841,14 @@
       <c r="Y59" s="5"/>
     </row>
     <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B60" s="11" t="s">
-        <v>416</v>
-      </c>
-      <c r="C60" s="11" t="s">
+      <c r="B60" s="12" t="s">
+        <v>460</v>
+      </c>
+      <c r="C60" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>171</v>
+        <v>142</v>
       </c>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
@@ -9474,10 +9873,10 @@
       <c r="Y60" s="5"/>
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B61" s="11" t="s">
-        <v>417</v>
-      </c>
-      <c r="C61" s="11" t="s">
+      <c r="B61" s="12" t="s">
+        <v>461</v>
+      </c>
+      <c r="C61" s="12" t="s">
         <v>16</v>
       </c>
       <c r="E61" s="5"/>
@@ -9503,10 +9902,10 @@
       <c r="Y61" s="5"/>
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B62" s="11" t="s">
-        <v>418</v>
-      </c>
-      <c r="C62" s="11" t="s">
+      <c r="B62" s="12" t="s">
+        <v>462</v>
+      </c>
+      <c r="C62" s="12" t="s">
         <v>42</v>
       </c>
       <c r="D62" s="0" t="s">
@@ -9535,14 +9934,14 @@
       <c r="Y62" s="5"/>
     </row>
     <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B63" s="11" t="s">
-        <v>419</v>
-      </c>
-      <c r="C63" s="11" t="s">
-        <v>42</v>
+      <c r="B63" s="12" t="s">
+        <v>463</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>231</v>
+        <v>289</v>
       </c>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
@@ -9567,14 +9966,11 @@
       <c r="Y63" s="5"/>
     </row>
     <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B64" s="11" t="s">
-        <v>420</v>
-      </c>
-      <c r="C64" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D64" s="0" t="s">
-        <v>62</v>
+      <c r="B64" s="12" t="s">
+        <v>464</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
@@ -9599,14 +9995,14 @@
       <c r="Y64" s="5"/>
     </row>
     <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B65" s="11" t="s">
-        <v>421</v>
-      </c>
-      <c r="C65" s="11" t="s">
-        <v>42</v>
+      <c r="B65" s="12" t="s">
+        <v>465</v>
+      </c>
+      <c r="C65" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>226</v>
+        <v>295</v>
       </c>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
@@ -9631,14 +10027,11 @@
       <c r="Y65" s="5"/>
     </row>
     <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B66" s="11" t="s">
-        <v>422</v>
-      </c>
-      <c r="C66" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D66" s="0" t="s">
-        <v>144</v>
+      <c r="B66" s="12" t="s">
+        <v>466</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
@@ -9663,14 +10056,14 @@
       <c r="Y66" s="5"/>
     </row>
     <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B67" s="11" t="s">
-        <v>423</v>
-      </c>
-      <c r="C67" s="11" t="s">
-        <v>26</v>
+      <c r="B67" s="12" t="s">
+        <v>467</v>
+      </c>
+      <c r="C67" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>214</v>
+        <v>57</v>
       </c>
       <c r="E67" s="5"/>
       <c r="F67" s="5"/>
@@ -9695,14 +10088,14 @@
       <c r="Y67" s="5"/>
     </row>
     <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B68" s="11" t="s">
-        <v>424</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>42</v>
+      <c r="B68" s="12" t="s">
+        <v>468</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>63</v>
+        <v>189</v>
       </c>
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
@@ -9727,14 +10120,11 @@
       <c r="Y68" s="5"/>
     </row>
     <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B69" s="11" t="s">
-        <v>425</v>
-      </c>
-      <c r="C69" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D69" s="0" t="s">
-        <v>63</v>
+      <c r="B69" s="12" t="s">
+        <v>469</v>
+      </c>
+      <c r="C69" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
@@ -9759,14 +10149,14 @@
       <c r="Y69" s="5"/>
     </row>
     <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B70" s="11" t="s">
-        <v>426</v>
-      </c>
-      <c r="C70" s="11" t="s">
+      <c r="B70" s="12" t="s">
+        <v>470</v>
+      </c>
+      <c r="C70" s="12" t="s">
         <v>42</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
@@ -9791,14 +10181,14 @@
       <c r="Y70" s="5"/>
     </row>
     <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B71" s="11" t="s">
-        <v>427</v>
-      </c>
-      <c r="C71" s="11" t="s">
+      <c r="B71" s="12" t="s">
+        <v>471</v>
+      </c>
+      <c r="C71" s="12" t="s">
         <v>42</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>219</v>
+        <v>249</v>
       </c>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
@@ -9823,14 +10213,14 @@
       <c r="Y71" s="5"/>
     </row>
     <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B72" s="11" t="s">
-        <v>428</v>
-      </c>
-      <c r="C72" s="11" t="s">
+      <c r="B72" s="12" t="s">
+        <v>472</v>
+      </c>
+      <c r="C72" s="12" t="s">
         <v>42</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>119</v>
+        <v>62</v>
       </c>
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
@@ -9855,14 +10245,14 @@
       <c r="Y72" s="5"/>
     </row>
     <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B73" s="11" t="s">
-        <v>429</v>
-      </c>
-      <c r="C73" s="11" t="s">
+      <c r="B73" s="12" t="s">
+        <v>473</v>
+      </c>
+      <c r="C73" s="12" t="s">
         <v>42</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>63</v>
+        <v>244</v>
       </c>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
@@ -9887,14 +10277,14 @@
       <c r="Y73" s="5"/>
     </row>
     <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B74" s="11" t="s">
-        <v>430</v>
-      </c>
-      <c r="C74" s="11" t="s">
-        <v>42</v>
+      <c r="B74" s="12" t="s">
+        <v>474</v>
+      </c>
+      <c r="C74" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>209</v>
+        <v>162</v>
       </c>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
@@ -9919,14 +10309,14 @@
       <c r="Y74" s="5"/>
     </row>
     <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B75" s="11" t="s">
-        <v>431</v>
-      </c>
-      <c r="C75" s="11" t="s">
-        <v>42</v>
+      <c r="B75" s="12" t="s">
+        <v>475</v>
+      </c>
+      <c r="C75" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>62</v>
+        <v>232</v>
       </c>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
@@ -9951,11 +10341,14 @@
       <c r="Y75" s="5"/>
     </row>
     <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B76" s="11" t="s">
-        <v>432</v>
-      </c>
-      <c r="C76" s="11" t="s">
-        <v>22</v>
+      <c r="B76" s="12" t="s">
+        <v>476</v>
+      </c>
+      <c r="C76" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>63</v>
       </c>
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
@@ -9980,14 +10373,14 @@
       <c r="Y76" s="5"/>
     </row>
     <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B77" s="11" t="s">
-        <v>433</v>
-      </c>
-      <c r="C77" s="11" t="s">
+      <c r="B77" s="12" t="s">
+        <v>477</v>
+      </c>
+      <c r="C77" s="12" t="s">
         <v>42</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="E77" s="5"/>
       <c r="F77" s="5"/>
@@ -10012,14 +10405,14 @@
       <c r="Y77" s="5"/>
     </row>
     <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B78" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="C78" s="11" t="s">
+      <c r="B78" s="12" t="s">
+        <v>478</v>
+      </c>
+      <c r="C78" s="12" t="s">
         <v>42</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>319</v>
+        <v>63</v>
       </c>
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
@@ -10044,14 +10437,14 @@
       <c r="Y78" s="5"/>
     </row>
     <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B79" s="11" t="s">
-        <v>434</v>
-      </c>
-      <c r="C79" s="11" t="s">
+      <c r="B79" s="12" t="s">
+        <v>479</v>
+      </c>
+      <c r="C79" s="12" t="s">
         <v>42</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>313</v>
+        <v>237</v>
       </c>
       <c r="E79" s="5"/>
       <c r="F79" s="5"/>
@@ -10076,14 +10469,14 @@
       <c r="Y79" s="5"/>
     </row>
     <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B80" s="11" t="s">
-        <v>435</v>
-      </c>
-      <c r="C80" s="11" t="s">
-        <v>26</v>
+      <c r="B80" s="12" t="s">
+        <v>480</v>
+      </c>
+      <c r="C80" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>92</v>
+        <v>137</v>
       </c>
       <c r="E80" s="5"/>
       <c r="F80" s="5"/>
@@ -10108,14 +10501,14 @@
       <c r="Y80" s="5"/>
     </row>
     <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B81" s="11" t="s">
-        <v>436</v>
-      </c>
-      <c r="C81" s="11" t="s">
+      <c r="B81" s="12" t="s">
+        <v>481</v>
+      </c>
+      <c r="C81" s="12" t="s">
         <v>42</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>308</v>
+        <v>63</v>
       </c>
       <c r="E81" s="5"/>
       <c r="F81" s="5"/>
@@ -10140,14 +10533,14 @@
       <c r="Y81" s="5"/>
     </row>
     <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B82" s="11" t="s">
-        <v>437</v>
-      </c>
-      <c r="C82" s="11" t="s">
+      <c r="B82" s="12" t="s">
+        <v>482</v>
+      </c>
+      <c r="C82" s="12" t="s">
         <v>42</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>320</v>
+        <v>227</v>
       </c>
       <c r="E82" s="5"/>
       <c r="F82" s="5"/>
@@ -10172,14 +10565,14 @@
       <c r="Y82" s="5"/>
     </row>
     <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B83" s="11" t="s">
-        <v>438</v>
-      </c>
-      <c r="C83" s="11" t="s">
-        <v>26</v>
+      <c r="B83" s="12" t="s">
+        <v>483</v>
+      </c>
+      <c r="C83" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>110</v>
+        <v>62</v>
       </c>
       <c r="E83" s="5"/>
       <c r="F83" s="5"/>
@@ -10204,14 +10597,11 @@
       <c r="Y83" s="5"/>
     </row>
     <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B84" s="11" t="s">
-        <v>439</v>
-      </c>
-      <c r="C84" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D84" s="0" t="s">
-        <v>57</v>
+      <c r="B84" s="12" t="s">
+        <v>484</v>
+      </c>
+      <c r="C84" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="E84" s="5"/>
       <c r="F84" s="5"/>
@@ -10236,14 +10626,14 @@
       <c r="Y84" s="5"/>
     </row>
     <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B85" s="11" t="s">
-        <v>321</v>
-      </c>
-      <c r="C85" s="11" t="s">
-        <v>26</v>
+      <c r="B85" s="12" t="s">
+        <v>485</v>
+      </c>
+      <c r="C85" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>321</v>
+        <v>27</v>
       </c>
       <c r="E85" s="5"/>
       <c r="F85" s="5"/>
@@ -10268,14 +10658,14 @@
       <c r="Y85" s="5"/>
     </row>
     <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B86" s="11" t="s">
-        <v>440</v>
-      </c>
-      <c r="C86" s="11" t="s">
+      <c r="B86" s="12" t="s">
+        <v>362</v>
+      </c>
+      <c r="C86" s="12" t="s">
         <v>42</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>66</v>
+        <v>362</v>
       </c>
       <c r="E86" s="5"/>
       <c r="F86" s="5"/>
@@ -10300,11 +10690,14 @@
       <c r="Y86" s="5"/>
     </row>
     <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B87" s="11" t="s">
-        <v>441</v>
-      </c>
-      <c r="C87" s="11" t="s">
-        <v>22</v>
+      <c r="B87" s="12" t="s">
+        <v>486</v>
+      </c>
+      <c r="C87" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D87" s="0" t="s">
+        <v>356</v>
       </c>
       <c r="E87" s="5"/>
       <c r="F87" s="5"/>
@@ -10329,6 +10722,15 @@
       <c r="Y87" s="5"/>
     </row>
     <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B88" s="12" t="s">
+        <v>487</v>
+      </c>
+      <c r="C88" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D88" s="0" t="s">
+        <v>92</v>
+      </c>
       <c r="E88" s="5"/>
       <c r="F88" s="5"/>
       <c r="G88" s="5"/>
@@ -10352,6 +10754,15 @@
       <c r="Y88" s="5"/>
     </row>
     <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B89" s="12" t="s">
+        <v>488</v>
+      </c>
+      <c r="C89" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D89" s="0" t="s">
+        <v>351</v>
+      </c>
       <c r="E89" s="5"/>
       <c r="F89" s="5"/>
       <c r="G89" s="5"/>
@@ -10375,6 +10786,15 @@
       <c r="Y89" s="5"/>
     </row>
     <row r="90" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B90" s="12" t="s">
+        <v>489</v>
+      </c>
+      <c r="C90" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D90" s="0" t="s">
+        <v>363</v>
+      </c>
       <c r="E90" s="5"/>
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
@@ -10398,6 +10818,15 @@
       <c r="Y90" s="5"/>
     </row>
     <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B91" s="12" t="s">
+        <v>490</v>
+      </c>
+      <c r="C91" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D91" s="0" t="s">
+        <v>110</v>
+      </c>
       <c r="E91" s="5"/>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
@@ -10421,6 +10850,15 @@
       <c r="Y91" s="5"/>
     </row>
     <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B92" s="12" t="s">
+        <v>491</v>
+      </c>
+      <c r="C92" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D92" s="0" t="s">
+        <v>57</v>
+      </c>
       <c r="E92" s="5"/>
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
@@ -10444,6 +10882,15 @@
       <c r="Y92" s="5"/>
     </row>
     <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B93" s="12" t="s">
+        <v>364</v>
+      </c>
+      <c r="C93" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D93" s="0" t="s">
+        <v>364</v>
+      </c>
       <c r="E93" s="5"/>
       <c r="F93" s="5"/>
       <c r="G93" s="5"/>
@@ -10467,6 +10914,15 @@
       <c r="Y93" s="5"/>
     </row>
     <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B94" s="12" t="s">
+        <v>492</v>
+      </c>
+      <c r="C94" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D94" s="0" t="s">
+        <v>66</v>
+      </c>
       <c r="E94" s="5"/>
       <c r="F94" s="5"/>
       <c r="G94" s="5"/>
@@ -10490,6 +10946,12 @@
       <c r="Y94" s="5"/>
     </row>
     <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B95" s="12" t="s">
+        <v>493</v>
+      </c>
+      <c r="C95" s="12" t="s">
+        <v>22</v>
+      </c>
       <c r="E95" s="5"/>
       <c r="F95" s="5"/>
       <c r="G95" s="5"/>
@@ -25255,7 +25717,7 @@
       <c r="X736" s="5"/>
       <c r="Y736" s="5"/>
     </row>
-    <row r="737" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="737" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E737" s="5"/>
       <c r="F737" s="5"/>
       <c r="G737" s="5"/>
@@ -25278,7 +25740,7 @@
       <c r="X737" s="5"/>
       <c r="Y737" s="5"/>
     </row>
-    <row r="738" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="738" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E738" s="5"/>
       <c r="F738" s="5"/>
       <c r="G738" s="5"/>
@@ -25301,7 +25763,7 @@
       <c r="X738" s="5"/>
       <c r="Y738" s="5"/>
     </row>
-    <row r="739" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="739" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E739" s="5"/>
       <c r="F739" s="5"/>
       <c r="G739" s="5"/>
@@ -25324,7 +25786,7 @@
       <c r="X739" s="5"/>
       <c r="Y739" s="5"/>
     </row>
-    <row r="740" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="740" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E740" s="5"/>
       <c r="F740" s="5"/>
       <c r="G740" s="5"/>
@@ -25347,7 +25809,7 @@
       <c r="X740" s="5"/>
       <c r="Y740" s="5"/>
     </row>
-    <row r="741" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="741" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E741" s="5"/>
       <c r="F741" s="5"/>
       <c r="G741" s="5"/>
@@ -25370,7 +25832,7 @@
       <c r="X741" s="5"/>
       <c r="Y741" s="5"/>
     </row>
-    <row r="742" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="742" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E742" s="5"/>
       <c r="F742" s="5"/>
       <c r="G742" s="5"/>
@@ -25393,7 +25855,7 @@
       <c r="X742" s="5"/>
       <c r="Y742" s="5"/>
     </row>
-    <row r="743" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="743" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E743" s="5"/>
       <c r="F743" s="5"/>
       <c r="G743" s="5"/>
@@ -25416,7 +25878,7 @@
       <c r="X743" s="5"/>
       <c r="Y743" s="5"/>
     </row>
-    <row r="744" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="744" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E744" s="5"/>
       <c r="F744" s="5"/>
       <c r="G744" s="5"/>
@@ -25508,6 +25970,190 @@
       <c r="X747" s="5"/>
       <c r="Y747" s="5"/>
     </row>
+    <row r="748" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E748" s="5"/>
+      <c r="F748" s="5"/>
+      <c r="G748" s="5"/>
+      <c r="H748" s="5"/>
+      <c r="I748" s="5"/>
+      <c r="J748" s="5"/>
+      <c r="K748" s="5"/>
+      <c r="L748" s="5"/>
+      <c r="M748" s="5"/>
+      <c r="N748" s="5"/>
+      <c r="O748" s="5"/>
+      <c r="P748" s="5"/>
+      <c r="Q748" s="5"/>
+      <c r="R748" s="5"/>
+      <c r="S748" s="5"/>
+      <c r="T748" s="5"/>
+      <c r="U748" s="5"/>
+      <c r="V748" s="5"/>
+      <c r="W748" s="5"/>
+      <c r="X748" s="5"/>
+      <c r="Y748" s="5"/>
+    </row>
+    <row r="749" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E749" s="5"/>
+      <c r="F749" s="5"/>
+      <c r="G749" s="5"/>
+      <c r="H749" s="5"/>
+      <c r="I749" s="5"/>
+      <c r="J749" s="5"/>
+      <c r="K749" s="5"/>
+      <c r="L749" s="5"/>
+      <c r="M749" s="5"/>
+      <c r="N749" s="5"/>
+      <c r="O749" s="5"/>
+      <c r="P749" s="5"/>
+      <c r="Q749" s="5"/>
+      <c r="R749" s="5"/>
+      <c r="S749" s="5"/>
+      <c r="T749" s="5"/>
+      <c r="U749" s="5"/>
+      <c r="V749" s="5"/>
+      <c r="W749" s="5"/>
+      <c r="X749" s="5"/>
+      <c r="Y749" s="5"/>
+    </row>
+    <row r="750" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E750" s="5"/>
+      <c r="F750" s="5"/>
+      <c r="G750" s="5"/>
+      <c r="H750" s="5"/>
+      <c r="I750" s="5"/>
+      <c r="J750" s="5"/>
+      <c r="K750" s="5"/>
+      <c r="L750" s="5"/>
+      <c r="M750" s="5"/>
+      <c r="N750" s="5"/>
+      <c r="O750" s="5"/>
+      <c r="P750" s="5"/>
+      <c r="Q750" s="5"/>
+      <c r="R750" s="5"/>
+      <c r="S750" s="5"/>
+      <c r="T750" s="5"/>
+      <c r="U750" s="5"/>
+      <c r="V750" s="5"/>
+      <c r="W750" s="5"/>
+      <c r="X750" s="5"/>
+      <c r="Y750" s="5"/>
+    </row>
+    <row r="751" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E751" s="5"/>
+      <c r="F751" s="5"/>
+      <c r="G751" s="5"/>
+      <c r="H751" s="5"/>
+      <c r="I751" s="5"/>
+      <c r="J751" s="5"/>
+      <c r="K751" s="5"/>
+      <c r="L751" s="5"/>
+      <c r="M751" s="5"/>
+      <c r="N751" s="5"/>
+      <c r="O751" s="5"/>
+      <c r="P751" s="5"/>
+      <c r="Q751" s="5"/>
+      <c r="R751" s="5"/>
+      <c r="S751" s="5"/>
+      <c r="T751" s="5"/>
+      <c r="U751" s="5"/>
+      <c r="V751" s="5"/>
+      <c r="W751" s="5"/>
+      <c r="X751" s="5"/>
+      <c r="Y751" s="5"/>
+    </row>
+    <row r="752" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E752" s="5"/>
+      <c r="F752" s="5"/>
+      <c r="G752" s="5"/>
+      <c r="H752" s="5"/>
+      <c r="I752" s="5"/>
+      <c r="J752" s="5"/>
+      <c r="K752" s="5"/>
+      <c r="L752" s="5"/>
+      <c r="M752" s="5"/>
+      <c r="N752" s="5"/>
+      <c r="O752" s="5"/>
+      <c r="P752" s="5"/>
+      <c r="Q752" s="5"/>
+      <c r="R752" s="5"/>
+      <c r="S752" s="5"/>
+      <c r="T752" s="5"/>
+      <c r="U752" s="5"/>
+      <c r="V752" s="5"/>
+      <c r="W752" s="5"/>
+      <c r="X752" s="5"/>
+      <c r="Y752" s="5"/>
+    </row>
+    <row r="753" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E753" s="5"/>
+      <c r="F753" s="5"/>
+      <c r="G753" s="5"/>
+      <c r="H753" s="5"/>
+      <c r="I753" s="5"/>
+      <c r="J753" s="5"/>
+      <c r="K753" s="5"/>
+      <c r="L753" s="5"/>
+      <c r="M753" s="5"/>
+      <c r="N753" s="5"/>
+      <c r="O753" s="5"/>
+      <c r="P753" s="5"/>
+      <c r="Q753" s="5"/>
+      <c r="R753" s="5"/>
+      <c r="S753" s="5"/>
+      <c r="T753" s="5"/>
+      <c r="U753" s="5"/>
+      <c r="V753" s="5"/>
+      <c r="W753" s="5"/>
+      <c r="X753" s="5"/>
+      <c r="Y753" s="5"/>
+    </row>
+    <row r="754" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E754" s="5"/>
+      <c r="F754" s="5"/>
+      <c r="G754" s="5"/>
+      <c r="H754" s="5"/>
+      <c r="I754" s="5"/>
+      <c r="J754" s="5"/>
+      <c r="K754" s="5"/>
+      <c r="L754" s="5"/>
+      <c r="M754" s="5"/>
+      <c r="N754" s="5"/>
+      <c r="O754" s="5"/>
+      <c r="P754" s="5"/>
+      <c r="Q754" s="5"/>
+      <c r="R754" s="5"/>
+      <c r="S754" s="5"/>
+      <c r="T754" s="5"/>
+      <c r="U754" s="5"/>
+      <c r="V754" s="5"/>
+      <c r="W754" s="5"/>
+      <c r="X754" s="5"/>
+      <c r="Y754" s="5"/>
+    </row>
+    <row r="755" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E755" s="5"/>
+      <c r="F755" s="5"/>
+      <c r="G755" s="5"/>
+      <c r="H755" s="5"/>
+      <c r="I755" s="5"/>
+      <c r="J755" s="5"/>
+      <c r="K755" s="5"/>
+      <c r="L755" s="5"/>
+      <c r="M755" s="5"/>
+      <c r="N755" s="5"/>
+      <c r="O755" s="5"/>
+      <c r="P755" s="5"/>
+      <c r="Q755" s="5"/>
+      <c r="R755" s="5"/>
+      <c r="S755" s="5"/>
+      <c r="T755" s="5"/>
+      <c r="U755" s="5"/>
+      <c r="V755" s="5"/>
+      <c r="W755" s="5"/>
+      <c r="X755" s="5"/>
+      <c r="Y755" s="5"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -25527,10 +26173,10 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:C4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.62890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.86"/>
@@ -25539,10 +26185,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>442</v>
+        <v>494</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>443</v>
+        <v>495</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>53</v>
@@ -25550,23 +26196,23 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>444</v>
+        <v>496</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>445</v>
+        <v>497</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>446</v>
+        <v>498</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>445</v>
+        <v>497</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>447</v>
+        <v>499</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>20210124001</v>
@@ -25574,15 +26220,15 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>448</v>
+        <v>500</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>449</v>
+        <v>501</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>450</v>
+        <v>502</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>

</xml_diff>